<commit_message>
add: add formula result
</commit_message>
<xml_diff>
--- a/first_process/data_o.xlsx
+++ b/first_process/data_o.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yuyouyu\SHU\BMG_Data_SHU\first_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70319C73-7209-4DDE-A8AA-FECB8A8D3A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13642DBE-162F-439E-8945-03D0A9388E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A7D8232-C0B1-467F-B589-3A6675527E49}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>Zr53Al16(Co0.75Ag0.25)31</t>
   </si>
   <si>
-    <t>Zr56Al16(Nio.7Ag0.3)28</t>
-  </si>
-  <si>
     <t>Zr53.5Cu26.5Ni5Al12Ag3</t>
   </si>
   <si>
@@ -532,6 +529,10 @@
   </si>
   <si>
     <t>Zr60Cu19Al10Ni10Ta1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zr56Al16(Ni0.7Ag0.3)28</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1030,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0E418F-30A3-42B6-B0DE-1476468B5902}">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:B69"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1063,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -1074,7 +1075,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="6">
         <v>7</v>
@@ -1114,7 +1115,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="6">
         <v>8.5</v>
@@ -1408,7 +1409,7 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="13">
         <v>18</v>
@@ -1482,7 +1483,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" s="13">
         <v>10</v>
@@ -1514,7 +1515,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="B23" s="13">
         <v>20</v>
@@ -1532,7 +1533,7 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="13">
         <v>20</v>
@@ -1550,7 +1551,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="13">
         <v>10</v>
@@ -1568,7 +1569,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1580,7 +1581,7 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="13">
         <v>50</v>
@@ -1598,7 +1599,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B28" s="13">
         <v>5</v>
@@ -1616,7 +1617,7 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B29" s="13">
         <v>5</v>
@@ -1640,7 +1641,7 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="13">
@@ -1662,7 +1663,7 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13">
@@ -1684,7 +1685,7 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13">
@@ -1706,7 +1707,7 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13">
@@ -1728,7 +1729,7 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B34" s="13">
         <v>5</v>
@@ -1742,7 +1743,7 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B35" s="13">
         <v>5</v>
@@ -1756,7 +1757,7 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36" s="13">
         <v>5</v>
@@ -1770,7 +1771,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="13">
         <v>3</v>
@@ -1784,7 +1785,7 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" s="13">
         <v>3</v>
@@ -1798,7 +1799,7 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B39" s="13">
         <v>3</v>
@@ -1812,7 +1813,7 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B40" s="13">
         <v>5</v>
@@ -1826,7 +1827,7 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B41" s="13">
         <v>3</v>
@@ -1840,7 +1841,7 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="13">
         <v>3</v>
@@ -1854,7 +1855,7 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" s="13">
         <v>3</v>
@@ -1868,7 +1869,7 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B44" s="8">
         <v>8</v>
@@ -1892,7 +1893,7 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B45" s="8">
         <v>8</v>
@@ -1916,7 +1917,7 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B46" s="8">
         <v>8</v>
@@ -1940,7 +1941,7 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B47" s="8">
         <v>8</v>
@@ -1964,7 +1965,7 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" s="8">
         <v>8</v>
@@ -1988,7 +1989,7 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" s="8">
         <v>8</v>
@@ -2012,7 +2013,7 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" s="8">
         <v>8</v>
@@ -2038,7 +2039,7 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" s="8">
         <v>8</v>
@@ -2064,7 +2065,7 @@
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" s="8">
         <v>8</v>
@@ -2090,7 +2091,7 @@
     </row>
     <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="8">
         <v>8</v>
@@ -2116,7 +2117,7 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" s="8">
         <v>8</v>
@@ -2142,7 +2143,7 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B55" s="8">
         <v>8</v>
@@ -2168,7 +2169,7 @@
     </row>
     <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B56" s="14">
         <v>2</v>
@@ -2192,7 +2193,7 @@
     </row>
     <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B57" s="7">
         <v>2</v>
@@ -2216,7 +2217,7 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B58" s="7">
         <v>2</v>
@@ -2240,7 +2241,7 @@
     </row>
     <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B59" s="15">
         <v>2</v>
@@ -2260,7 +2261,7 @@
     </row>
     <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B60" s="15">
         <v>2</v>
@@ -2280,7 +2281,7 @@
     </row>
     <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B61" s="16">
         <v>8</v>
@@ -2306,7 +2307,7 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B62" s="6">
         <v>8</v>
@@ -2332,7 +2333,7 @@
     </row>
     <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B63" s="6">
         <v>8</v>
@@ -2358,7 +2359,7 @@
     </row>
     <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B64" s="6">
         <v>8</v>
@@ -2384,7 +2385,7 @@
     </row>
     <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B65" s="17">
         <v>8</v>
@@ -2410,7 +2411,7 @@
     </row>
     <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B66" s="17">
         <v>8</v>
@@ -2436,7 +2437,7 @@
     </row>
     <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67" s="14">
         <v>3</v>
@@ -2458,7 +2459,7 @@
     </row>
     <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B68" s="8">
         <v>3</v>
@@ -2480,7 +2481,7 @@
     </row>
     <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B69" s="8">
         <v>3</v>
@@ -2502,7 +2503,7 @@
     </row>
     <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B70" s="13">
         <v>3</v>
@@ -2524,7 +2525,7 @@
     </row>
     <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B71" s="13">
         <v>3</v>
@@ -2546,7 +2547,7 @@
     </row>
     <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B72" s="13">
         <v>3</v>
@@ -2568,7 +2569,7 @@
     </row>
     <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B73" s="13">
         <v>3</v>
@@ -2590,7 +2591,7 @@
     </row>
     <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B74" s="8">
         <v>5</v>
@@ -2610,7 +2611,7 @@
     </row>
     <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B75" s="11">
         <v>15</v>
@@ -2634,7 +2635,7 @@
     </row>
     <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B76" s="19">
         <v>12</v>
@@ -2658,7 +2659,7 @@
     </row>
     <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B77" s="19">
         <v>8</v>
@@ -2678,7 +2679,7 @@
     </row>
     <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B78" s="13">
         <v>10</v>
@@ -2702,7 +2703,7 @@
     </row>
     <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B79" s="13">
         <v>4.2</v>
@@ -2718,7 +2719,7 @@
     </row>
     <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B80" s="13">
         <v>8</v>
@@ -2734,7 +2735,7 @@
     </row>
     <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B81" s="13">
         <v>2</v>
@@ -2750,7 +2751,7 @@
     </row>
     <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B82" s="13">
         <v>10</v>
@@ -2766,7 +2767,7 @@
     </row>
     <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B83" s="13">
         <v>2</v>
@@ -2782,7 +2783,7 @@
     </row>
     <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -2796,7 +2797,7 @@
     </row>
     <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -2810,7 +2811,7 @@
     </row>
     <row r="86" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -2824,7 +2825,7 @@
     </row>
     <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -2838,7 +2839,7 @@
     </row>
     <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B88" s="11">
         <v>20</v>
@@ -2858,7 +2859,7 @@
     </row>
     <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B89" s="13">
         <v>11</v>
@@ -2878,7 +2879,7 @@
     </row>
     <row r="90" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B90" s="13">
         <v>25</v>
@@ -2898,7 +2899,7 @@
     </row>
     <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B91" s="13">
         <v>9</v>
@@ -2918,7 +2919,7 @@
     </row>
     <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B92" s="13">
         <v>18</v>
@@ -2936,7 +2937,7 @@
     </row>
     <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B93" s="13">
         <v>10</v>
@@ -2956,7 +2957,7 @@
     </row>
     <row r="94" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B94" s="13">
         <v>30</v>
@@ -2976,7 +2977,7 @@
     </row>
     <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B95" s="13">
         <v>1.5</v>
@@ -2996,7 +2997,7 @@
     </row>
     <row r="96" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B96" s="13">
         <v>3</v>
@@ -3016,7 +3017,7 @@
     </row>
     <row r="97" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B97" s="11">
         <v>12</v>
@@ -3034,7 +3035,7 @@
     </row>
     <row r="98" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B98" s="13">
         <v>5</v>
@@ -3052,7 +3053,7 @@
     </row>
     <row r="99" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B99" s="13">
         <v>14</v>
@@ -3068,7 +3069,7 @@
     </row>
     <row r="100" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B100" s="13">
         <v>20</v>
@@ -3082,7 +3083,7 @@
     </row>
     <row r="101" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B101" s="13">
         <v>20</v>
@@ -3100,7 +3101,7 @@
     </row>
     <row r="102" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B102" s="11">
         <v>10</v>
@@ -3126,7 +3127,7 @@
     </row>
     <row r="103" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B103" s="13">
         <v>10</v>
@@ -3152,7 +3153,7 @@
     </row>
     <row r="104" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B104" s="13">
         <v>10</v>
@@ -3178,7 +3179,7 @@
     </row>
     <row r="105" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B105" s="13">
         <v>10</v>
@@ -3204,7 +3205,7 @@
     </row>
     <row r="106" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B106" s="8">
         <v>3</v>
@@ -3226,7 +3227,7 @@
     </row>
     <row r="107" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B107" s="8">
         <v>4</v>
@@ -3248,7 +3249,7 @@
     </row>
     <row r="108" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B108" s="8">
         <v>4</v>
@@ -3270,7 +3271,7 @@
     </row>
     <row r="109" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B109" s="8">
         <v>4</v>
@@ -3292,7 +3293,7 @@
     </row>
     <row r="110" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B110" s="8">
         <v>3</v>
@@ -3312,7 +3313,7 @@
     </row>
     <row r="111" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B111" s="8">
         <v>2</v>
@@ -3336,7 +3337,7 @@
     </row>
     <row r="112" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B112" s="8">
         <v>2</v>
@@ -3360,7 +3361,7 @@
     </row>
     <row r="113" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B113" s="8">
         <v>2</v>
@@ -3384,7 +3385,7 @@
     </row>
     <row r="114" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B114" s="8">
         <v>2</v>
@@ -3408,7 +3409,7 @@
     </row>
     <row r="115" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B115" s="8">
         <v>2</v>
@@ -3432,7 +3433,7 @@
     </row>
     <row r="116" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" s="11">
         <v>73</v>
@@ -3454,7 +3455,7 @@
     </row>
     <row r="117" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B117" s="13">
         <v>35</v>
@@ -3476,7 +3477,7 @@
     </row>
     <row r="118" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B118" s="13"/>
       <c r="C118" s="13">
@@ -3496,7 +3497,7 @@
     </row>
     <row r="119" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B119" s="13"/>
       <c r="C119" s="13">
@@ -3516,7 +3517,7 @@
     </row>
     <row r="120" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B120" s="13"/>
       <c r="C120" s="13">
@@ -3536,7 +3537,7 @@
     </row>
     <row r="121" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B121" s="13">
         <v>52</v>
@@ -3558,7 +3559,7 @@
     </row>
     <row r="122" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B122" s="13"/>
       <c r="C122" s="13">
@@ -3578,7 +3579,7 @@
     </row>
     <row r="123" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B123" s="13"/>
       <c r="C123" s="13">
@@ -3598,7 +3599,7 @@
     </row>
     <row r="124" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B124" s="21">
         <v>12.6</v>
@@ -3622,7 +3623,7 @@
     </row>
     <row r="125" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B125" s="8">
         <v>16</v>
@@ -3646,7 +3647,7 @@
     </row>
     <row r="126" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B126" s="8">
         <v>4</v>
@@ -3668,7 +3669,7 @@
     </row>
     <row r="127" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B127" s="8">
         <v>4</v>
@@ -3688,7 +3689,7 @@
     </row>
     <row r="128" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B128" s="8">
         <v>4</v>
@@ -3708,7 +3709,7 @@
     </row>
     <row r="129" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B129" s="8">
         <v>4</v>
@@ -3728,7 +3729,7 @@
     </row>
     <row r="130" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B130" s="8">
         <v>4</v>
@@ -3748,7 +3749,7 @@
     </row>
     <row r="131" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B131" s="8">
         <v>4</v>
@@ -3768,7 +3769,7 @@
     </row>
     <row r="132" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B132" s="8">
         <v>4</v>
@@ -3788,7 +3789,7 @@
     </row>
     <row r="133" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B133" s="8">
         <v>4</v>
@@ -3808,7 +3809,7 @@
     </row>
     <row r="134" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B134" s="8">
         <v>6</v>
@@ -3832,7 +3833,7 @@
     </row>
     <row r="135" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B135" s="8">
         <v>10</v>
@@ -3874,7 +3875,7 @@
     </row>
     <row r="137" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B137" s="14">
         <v>16</v>
@@ -3898,7 +3899,7 @@
     </row>
     <row r="138" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B138" s="13"/>
       <c r="C138" s="13"/>
@@ -3912,7 +3913,7 @@
     </row>
     <row r="139" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B139" s="7">
         <v>30</v>
@@ -3936,7 +3937,7 @@
     </row>
     <row r="140" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B140" s="6">
         <v>14</v>
@@ -3956,7 +3957,7 @@
     </row>
     <row r="141" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B141" s="6">
         <v>14</v>
@@ -3976,7 +3977,7 @@
     </row>
     <row r="142" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B142" s="6">
         <v>3</v>
@@ -4000,7 +4001,7 @@
     </row>
     <row r="143" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B143" s="8">
         <v>30</v>
@@ -4022,7 +4023,7 @@
     </row>
     <row r="144" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B144" s="6">
         <v>2</v>

</xml_diff>